<commit_message>
Station - Add station implemented
</commit_message>
<xml_diff>
--- a/data_sheets/london.xlsx
+++ b/data_sheets/london.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\tubemaphistory\tube-map-history.api\data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A701D9-92EB-4D67-B7A7-F4E8C40EBC25}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60721F98-380D-4C57-9DC2-B7A18E812494}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="18" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="673">
   <si>
     <t>name</t>
   </si>
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B57CB05-6C06-4E09-A4F6-BAF5C3308C96}">
   <dimension ref="A1:E610"/>
   <sheetViews>
-    <sheetView topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9978,10 +9978,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10077,6 +10077,70 @@
         <v>1863</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J9">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>390</v>
+      </c>
+      <c r="J12">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>436</v>
+      </c>
+      <c r="J13">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>588</v>
+      </c>
+      <c r="J14">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>309</v>
+      </c>
+      <c r="J15">
+        <v>1864</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -10087,10 +10151,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:J7"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10205,6 +10269,70 @@
       </c>
       <c r="J7">
         <v>1863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J9">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>390</v>
+      </c>
+      <c r="J12">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>436</v>
+      </c>
+      <c r="J13">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>588</v>
+      </c>
+      <c r="J14">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>309</v>
+      </c>
+      <c r="J15">
+        <v>1864</v>
       </c>
     </row>
   </sheetData>
@@ -13891,10 +14019,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13991,6 +14119,46 @@
         <v>1863</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J9">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>199</v>
+      </c>
+      <c r="J11">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>568</v>
+      </c>
+      <c r="J12">
+        <v>1894</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>